<commit_message>
integrating lcd and flow sensor
met some interruption issue. solution see code.
</commit_message>
<xml_diff>
--- a/FlowSensorPID/experiments.xlsx
+++ b/FlowSensorPID/experiments.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="-21160" windowWidth="24940" windowHeight="16760" tabRatio="500"/>
+    <workbookView xWindow="9580" yWindow="440" windowWidth="19000" windowHeight="16760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
   <si>
     <t>defRate</t>
   </si>
@@ -108,6 +108,18 @@
   </si>
   <si>
     <t>kp/(tan(double(dT)/40.0)*180.0)</t>
+  </si>
+  <si>
+    <t>kp*tan(x/50)</t>
+  </si>
+  <si>
+    <t>kp*tan((x+10)/65)</t>
+  </si>
+  <si>
+    <t>kp*tan((x+5)/65)</t>
+  </si>
+  <si>
+    <t>kp*tan((x+7)/65)</t>
   </si>
 </sst>
 </file>
@@ -116,7 +128,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="167" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -181,10 +193,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -468,11 +480,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K56"/>
+  <dimension ref="A1:K66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D56" sqref="D56"/>
+      <selection pane="bottomLeft" activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -536,7 +548,7 @@
         <v>190</v>
       </c>
       <c r="G2" s="3">
-        <f>D2/F2</f>
+        <f t="shared" ref="G2:G39" si="0">D2/F2</f>
         <v>0.13157894736842105</v>
       </c>
       <c r="H2" s="3">
@@ -544,7 +556,7 @@
         <v>0.11889473684210526</v>
       </c>
       <c r="I2" s="5">
-        <f>(D2-E2)/D2</f>
+        <f t="shared" ref="I2:I39" si="1">(D2-E2)/D2</f>
         <v>9.64E-2</v>
       </c>
     </row>
@@ -569,15 +581,15 @@
         <v>211</v>
       </c>
       <c r="G3" s="3">
-        <f>D3/F3</f>
+        <f t="shared" si="0"/>
         <v>0.14218009478672985</v>
       </c>
       <c r="H3" s="3">
-        <f t="shared" ref="H3:H39" si="0">E3/F3</f>
+        <f t="shared" ref="H3:H39" si="2">E3/F3</f>
         <v>0.13251184834123222</v>
       </c>
       <c r="I3" s="5">
-        <f>(D3-E3)/D3</f>
+        <f t="shared" si="1"/>
         <v>6.7999999999999977E-2</v>
       </c>
     </row>
@@ -602,21 +614,21 @@
         <v>180</v>
       </c>
       <c r="G4" s="3">
-        <f>D4/F4</f>
+        <f t="shared" si="0"/>
         <v>0.12222222222222222</v>
       </c>
       <c r="H4" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.13355555555555554</v>
       </c>
       <c r="I4" s="5">
-        <f>(D4-E4)/D4</f>
+        <f t="shared" si="1"/>
         <v>-9.2727272727272686E-2</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
-        <f t="shared" ref="A5:A9" si="1">2/17</f>
+        <f t="shared" ref="A5:A9" si="3">2/17</f>
         <v>0.11764705882352941</v>
       </c>
       <c r="B5">
@@ -635,15 +647,15 @@
         <v>340</v>
       </c>
       <c r="G5" s="3">
-        <f>D5/F5</f>
+        <f t="shared" si="0"/>
         <v>0.11470588235294117</v>
       </c>
       <c r="H5" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.13223529411764706</v>
       </c>
       <c r="I5" s="5">
-        <f>(D5-E5)/D5</f>
+        <f t="shared" si="1"/>
         <v>-0.15282051282051284</v>
       </c>
       <c r="J5" t="s">
@@ -652,7 +664,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.11764705882352941</v>
       </c>
       <c r="B6">
@@ -671,15 +683,15 @@
         <v>347</v>
       </c>
       <c r="G6" s="3">
-        <f>D6/F6</f>
+        <f t="shared" si="0"/>
         <v>0.12968299711815562</v>
       </c>
       <c r="H6" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.13051873198847261</v>
       </c>
       <c r="I6" s="5">
-        <f>(D6-E6)/D6</f>
+        <f t="shared" si="1"/>
         <v>-6.4444444444444254E-3</v>
       </c>
       <c r="J6" t="s">
@@ -688,7 +700,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.11764705882352941</v>
       </c>
       <c r="B7">
@@ -707,15 +719,15 @@
         <v>330</v>
       </c>
       <c r="G7" s="3">
-        <f>D7/F7</f>
+        <f t="shared" si="0"/>
         <v>0.11212121212121212</v>
       </c>
       <c r="H7" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.13175757575757574</v>
       </c>
       <c r="I7" s="5">
-        <f>(D7-E7)/D7</f>
+        <f t="shared" si="1"/>
         <v>-0.17513513513513504</v>
       </c>
       <c r="J7" t="s">
@@ -724,7 +736,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.11764705882352941</v>
       </c>
       <c r="B8">
@@ -743,15 +755,15 @@
         <v>253</v>
       </c>
       <c r="G8" s="3">
-        <f>D8/F8</f>
+        <f t="shared" si="0"/>
         <v>0.15019762845849802</v>
       </c>
       <c r="H8" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.14588932806324109</v>
       </c>
       <c r="I8" s="5">
-        <f>(D8-E8)/D8</f>
+        <f t="shared" si="1"/>
         <v>2.8684210526315878E-2</v>
       </c>
       <c r="J8" t="s">
@@ -760,7 +772,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.11764705882352941</v>
       </c>
       <c r="B9">
@@ -779,15 +791,15 @@
         <v>353</v>
       </c>
       <c r="G9" s="3">
-        <f>D9/F9</f>
+        <f t="shared" si="0"/>
         <v>0.11331444759206799</v>
       </c>
       <c r="H9" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.13640226628895183</v>
       </c>
       <c r="I9" s="5">
-        <f>(D9-E9)/D9</f>
+        <f t="shared" si="1"/>
         <v>-0.20374999999999996</v>
       </c>
       <c r="J9" t="s">
@@ -815,15 +827,15 @@
         <v>313</v>
       </c>
       <c r="G10" s="3">
-        <f>D10/F10</f>
+        <f t="shared" si="0"/>
         <v>0.13418530351437699</v>
       </c>
       <c r="H10" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.11638977635782748</v>
       </c>
       <c r="I10" s="5">
-        <f>(D10-E10)/D10</f>
+        <f t="shared" si="1"/>
         <v>0.13261904761904764</v>
       </c>
       <c r="J10" t="s">
@@ -832,7 +844,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
-        <f t="shared" ref="A11:A17" si="2">3/20</f>
+        <f t="shared" ref="A11:A17" si="4">3/20</f>
         <v>0.15</v>
       </c>
       <c r="B11">
@@ -851,15 +863,15 @@
         <v>303</v>
       </c>
       <c r="G11" s="3">
-        <f>D11/F11</f>
+        <f t="shared" si="0"/>
         <v>0.12871287128712872</v>
       </c>
       <c r="H11" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.13029702970297027</v>
       </c>
       <c r="I11" s="5">
-        <f>(D11-E11)/D11</f>
+        <f t="shared" si="1"/>
         <v>-1.2307692307692228E-2</v>
       </c>
       <c r="J11" t="s">
@@ -868,7 +880,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.15</v>
       </c>
       <c r="B12">
@@ -887,15 +899,15 @@
         <v>357</v>
       </c>
       <c r="G12" s="3">
-        <f>D12/F12</f>
+        <f t="shared" si="0"/>
         <v>0.11204481792717087</v>
       </c>
       <c r="H12" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.11420168067226892</v>
       </c>
       <c r="I12" s="5">
-        <f>(D12-E12)/D12</f>
+        <f t="shared" si="1"/>
         <v>-1.925000000000008E-2</v>
       </c>
       <c r="J12" t="s">
@@ -904,7 +916,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.15</v>
       </c>
       <c r="B13">
@@ -923,15 +935,15 @@
         <v>200</v>
       </c>
       <c r="G13" s="3">
-        <f>D13/F13</f>
+        <f t="shared" si="0"/>
         <v>0.12</v>
       </c>
       <c r="H13" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.11244999999999999</v>
       </c>
       <c r="I13" s="5">
-        <f>(D13-E13)/D13</f>
+        <f t="shared" si="1"/>
         <v>6.2916666666666732E-2</v>
       </c>
       <c r="J13" t="s">
@@ -940,7 +952,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.15</v>
       </c>
       <c r="B14">
@@ -959,21 +971,21 @@
         <v>313</v>
       </c>
       <c r="G14" s="3">
-        <f>D14/F14</f>
+        <f t="shared" si="0"/>
         <v>0.11501597444089456</v>
       </c>
       <c r="H14" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.11166134185303515</v>
       </c>
       <c r="I14" s="5">
-        <f>(D14-E14)/D14</f>
+        <f t="shared" si="1"/>
         <v>2.9166666666666587E-2</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.15</v>
       </c>
       <c r="B15">
@@ -992,21 +1004,21 @@
         <v>164</v>
       </c>
       <c r="G15" s="3">
-        <f>D15/F15</f>
+        <f t="shared" si="0"/>
         <v>0.13414634146341464</v>
       </c>
       <c r="H15" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.11908536585365855</v>
       </c>
       <c r="I15" s="6">
-        <f>(D15-E15)/D15</f>
+        <f t="shared" si="1"/>
         <v>0.11227272727272722</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.15</v>
       </c>
       <c r="B16" s="1">
@@ -1025,22 +1037,22 @@
         <v>108</v>
       </c>
       <c r="G16" s="4">
-        <f>D16/F16</f>
+        <f t="shared" si="0"/>
         <v>0.15740740740740741</v>
       </c>
       <c r="H16" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.12722222222222224</v>
       </c>
       <c r="I16" s="7">
-        <f>(D16-E16)/D16</f>
+        <f t="shared" si="1"/>
         <v>0.19176470588235292</v>
       </c>
       <c r="J16" s="1"/>
     </row>
     <row r="17" spans="1:11" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.15</v>
       </c>
       <c r="B17">
@@ -1057,15 +1069,15 @@
         <v>24</v>
       </c>
       <c r="G17" s="3">
-        <f>D17/F17</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H17" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.17208333333333334</v>
       </c>
       <c r="I17" s="6" t="e">
-        <f>(D17-E17)/D17</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J17" t="s">
@@ -1096,21 +1108,21 @@
         <v>115</v>
       </c>
       <c r="G18" s="3">
-        <f>D18/F18</f>
+        <f t="shared" si="0"/>
         <v>0.18260869565217391</v>
       </c>
       <c r="H18" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.14721739130434783</v>
       </c>
       <c r="I18" s="6">
-        <f>(D18-E18)/D18</f>
+        <f t="shared" si="1"/>
         <v>0.19380952380952382</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19">
-        <f t="shared" ref="A19:A23" si="3">3/20</f>
+        <f t="shared" ref="A19:A23" si="5">3/20</f>
         <v>0.15</v>
       </c>
       <c r="B19">
@@ -1126,21 +1138,21 @@
         <v>107</v>
       </c>
       <c r="G19" s="3">
-        <f>D19/F19</f>
+        <f t="shared" si="0"/>
         <v>0.20560747663551401</v>
       </c>
       <c r="H19" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I19" s="6">
-        <f>(D19-E19)/D19</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.15</v>
       </c>
       <c r="B20">
@@ -1159,21 +1171,21 @@
         <v>97</v>
       </c>
       <c r="G20" s="3">
-        <f>D20/F20</f>
+        <f t="shared" si="0"/>
         <v>0.37113402061855671</v>
       </c>
       <c r="H20" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.19154639175257729</v>
       </c>
       <c r="I20" s="6">
-        <f>(D20-E20)/D20</f>
+        <f t="shared" si="1"/>
         <v>0.48388888888888892</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.15</v>
       </c>
       <c r="B21">
@@ -1192,21 +1204,21 @@
         <v>184</v>
       </c>
       <c r="G21" s="3">
-        <f>D21/F21</f>
+        <f t="shared" si="0"/>
         <v>0.20652173913043478</v>
       </c>
       <c r="H21" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.17766304347826087</v>
       </c>
       <c r="I21" s="6">
-        <f>(D21-E21)/D21</f>
+        <f t="shared" si="1"/>
         <v>0.13973684210526321</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.15</v>
       </c>
       <c r="B22">
@@ -1222,21 +1234,21 @@
         <v>309</v>
       </c>
       <c r="G22" s="3">
-        <f>D22/F22</f>
+        <f t="shared" si="0"/>
         <v>0.14886731391585761</v>
       </c>
       <c r="H22" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I22" s="6">
-        <f>(D22-E22)/D22</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.15</v>
       </c>
       <c r="B23">
@@ -1255,15 +1267,15 @@
         <v>509</v>
       </c>
       <c r="G23" s="3">
-        <f>D23/F23</f>
+        <f t="shared" si="0"/>
         <v>9.4302554027504912E-2</v>
       </c>
       <c r="H23" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.11787819253438114</v>
       </c>
       <c r="I23" s="6">
-        <f>(D23-E23)/D23</f>
+        <f t="shared" si="1"/>
         <v>-0.25</v>
       </c>
       <c r="J23" t="s">
@@ -1290,15 +1302,15 @@
         <v>430</v>
       </c>
       <c r="G24" s="3">
-        <f>D24/F24</f>
+        <f t="shared" si="0"/>
         <v>0.1186046511627907</v>
       </c>
       <c r="H24" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.15062790697674416</v>
       </c>
       <c r="I24" s="6">
-        <f>(D24-E24)/D24</f>
+        <f t="shared" si="1"/>
         <v>-0.26999999999999991</v>
       </c>
     </row>
@@ -1322,15 +1334,15 @@
         <v>298</v>
       </c>
       <c r="G25" s="3">
-        <f>D25/F25</f>
+        <f t="shared" si="0"/>
         <v>0.10067114093959731</v>
       </c>
       <c r="H25" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.13906040268456374</v>
       </c>
       <c r="I25" s="6">
-        <f>(D25-E25)/D25</f>
+        <f t="shared" si="1"/>
         <v>-0.38133333333333325</v>
       </c>
     </row>
@@ -1354,15 +1366,15 @@
         <v>258</v>
       </c>
       <c r="G26" s="3">
-        <f>D26/F26</f>
+        <f t="shared" si="0"/>
         <v>9.6899224806201556E-2</v>
       </c>
       <c r="H26" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.1160077519379845</v>
       </c>
       <c r="I26" s="6">
-        <f>(D26-E26)/D26</f>
+        <f t="shared" si="1"/>
         <v>-0.19719999999999999</v>
       </c>
       <c r="J26" t="s">
@@ -1389,15 +1401,15 @@
         <v>202</v>
       </c>
       <c r="G27" s="3">
-        <f>D27/F27</f>
+        <f t="shared" si="0"/>
         <v>0.11386138613861387</v>
       </c>
       <c r="H27" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.13133663366336634</v>
       </c>
       <c r="I27" s="6">
-        <f>(D27-E27)/D27</f>
+        <f t="shared" si="1"/>
         <v>-0.15347826086956526</v>
       </c>
     </row>
@@ -1421,15 +1433,15 @@
         <v>188</v>
       </c>
       <c r="G28" s="3">
-        <f>D28/F28</f>
+        <f t="shared" si="0"/>
         <v>0.12234042553191489</v>
       </c>
       <c r="H28" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9.8297872340425529E-2</v>
       </c>
       <c r="I28" s="6">
-        <f>(D28-E28)/D28</f>
+        <f t="shared" si="1"/>
         <v>0.19652173913043477</v>
       </c>
       <c r="J28" t="s">
@@ -1456,15 +1468,15 @@
         <v>175</v>
       </c>
       <c r="G29" s="3">
-        <f>D29/F29</f>
+        <f t="shared" si="0"/>
         <v>0.17714285714285713</v>
       </c>
       <c r="H29" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.13337142857142856</v>
       </c>
       <c r="I29" s="6">
-        <f>(D29-E29)/D29</f>
+        <f t="shared" si="1"/>
         <v>0.24709677419354839</v>
       </c>
     </row>
@@ -1485,15 +1497,15 @@
         <v>300</v>
       </c>
       <c r="G30" s="3">
-        <f>D30/F30</f>
+        <f t="shared" si="0"/>
         <v>0.10666666666666667</v>
       </c>
       <c r="H30" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I30" s="6">
-        <f>(D30-E30)/D30</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J30" t="s">
@@ -1520,15 +1532,15 @@
         <v>270</v>
       </c>
       <c r="G31" s="3">
-        <f>D31/F31</f>
+        <f t="shared" si="0"/>
         <v>0.11851851851851852</v>
       </c>
       <c r="H31" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.18059259259259258</v>
       </c>
       <c r="I31" s="8">
-        <f>(D31-E31)/D31</f>
+        <f t="shared" si="1"/>
         <v>-0.52374999999999994</v>
       </c>
       <c r="J31" t="s">
@@ -1555,15 +1567,15 @@
         <v>276</v>
       </c>
       <c r="G32" s="3">
-        <f>D32/F32</f>
+        <f t="shared" si="0"/>
         <v>0.11594202898550725</v>
       </c>
       <c r="H32" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.1665942028985507</v>
       </c>
       <c r="I32" s="8">
-        <f>(D32-E32)/D32</f>
+        <f t="shared" si="1"/>
         <v>-0.4368749999999999</v>
       </c>
       <c r="J32" t="s">
@@ -1590,15 +1602,15 @@
         <v>273</v>
       </c>
       <c r="G33" s="3">
-        <f>D33/F33</f>
+        <f t="shared" si="0"/>
         <v>0.10622710622710622</v>
       </c>
       <c r="H33" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.12758241758241759</v>
       </c>
       <c r="I33" s="8">
-        <f>(D33-E33)/D33</f>
+        <f t="shared" si="1"/>
         <v>-0.20103448275862063</v>
       </c>
     </row>
@@ -1622,15 +1634,15 @@
         <v>279</v>
       </c>
       <c r="G34" s="3">
-        <f>D34/F34</f>
+        <f t="shared" si="0"/>
         <v>0.11827956989247312</v>
       </c>
       <c r="H34" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.11279569892473118</v>
       </c>
       <c r="I34" s="8">
-        <f>(D34-E34)/D34</f>
+        <f t="shared" si="1"/>
         <v>4.6363636363636399E-2</v>
       </c>
     </row>
@@ -1654,15 +1666,15 @@
         <v>313</v>
       </c>
       <c r="G35" s="3">
-        <f>D35/F35</f>
+        <f t="shared" si="0"/>
         <v>0.11182108626198083</v>
       </c>
       <c r="H35" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.1006709265175719</v>
       </c>
       <c r="I35" s="8">
-        <f>(D35-E35)/D35</f>
+        <f t="shared" si="1"/>
         <v>9.9714285714285672E-2</v>
       </c>
     </row>
@@ -1686,15 +1698,15 @@
         <v>382</v>
       </c>
       <c r="G36" s="3">
-        <f>D36/F36</f>
+        <f t="shared" si="0"/>
         <v>9.9162303664921472E-2</v>
       </c>
       <c r="H36" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9.947643979057591E-2</v>
       </c>
       <c r="I36" s="8">
-        <f>(D36-E36)/D36</f>
+        <f t="shared" si="1"/>
         <v>-3.1678986272438603E-3</v>
       </c>
     </row>
@@ -1718,15 +1730,15 @@
         <v>100</v>
       </c>
       <c r="G37" s="3">
-        <f>D37/F37</f>
+        <f t="shared" si="0"/>
         <v>0.28999999999999998</v>
       </c>
       <c r="H37" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.1714</v>
       </c>
       <c r="I37" s="8">
-        <f>(D37-E37)/D37</f>
+        <f t="shared" si="1"/>
         <v>0.40896551724137931</v>
       </c>
       <c r="J37" t="s">
@@ -1753,15 +1765,15 @@
         <v>73</v>
       </c>
       <c r="G38" s="3">
-        <f>D38/F38</f>
+        <f t="shared" si="0"/>
         <v>0.43835616438356162</v>
       </c>
       <c r="H38" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.17027397260273971</v>
       </c>
       <c r="I38" s="8">
-        <f>(D38-E38)/D38</f>
+        <f t="shared" si="1"/>
         <v>0.61156250000000001</v>
       </c>
       <c r="J38" t="s">
@@ -1788,15 +1800,15 @@
         <v>167</v>
       </c>
       <c r="G39" s="3">
-        <f>D39/F39</f>
+        <f t="shared" si="0"/>
         <v>0.19161676646706588</v>
       </c>
       <c r="H39" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.1497005988023952</v>
       </c>
       <c r="I39" s="8">
-        <f>(D39-E39)/D39</f>
+        <f t="shared" si="1"/>
         <v>0.21875</v>
       </c>
       <c r="J39" t="s">
@@ -1823,15 +1835,15 @@
         <v>338</v>
       </c>
       <c r="G40" s="3">
-        <f t="shared" ref="G40:G47" si="4">D40/F40</f>
+        <f t="shared" ref="G40:G47" si="6">D40/F40</f>
         <v>0.11538461538461539</v>
       </c>
       <c r="H40" s="3">
-        <f t="shared" ref="H40:H47" si="5">E40/F40</f>
+        <f t="shared" ref="H40:H47" si="7">E40/F40</f>
         <v>5.8579881656804736E-2</v>
       </c>
       <c r="I40" s="8">
-        <f t="shared" ref="I40:I47" si="6">(D40-E40)/D40</f>
+        <f t="shared" ref="I40:I47" si="8">(D40-E40)/D40</f>
         <v>0.49230769230769228</v>
       </c>
       <c r="J40" t="s">
@@ -1855,15 +1867,15 @@
         <v>26.17</v>
       </c>
       <c r="G41" s="3" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H41" s="3" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I41" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.2730555555555555</v>
       </c>
       <c r="J41" t="s">
@@ -1960,15 +1972,15 @@
         <v>316</v>
       </c>
       <c r="G44" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.11075949367088607</v>
       </c>
       <c r="H44" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.15917721518987341</v>
       </c>
       <c r="I44" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-0.43714285714285706</v>
       </c>
       <c r="J44" t="s">
@@ -1995,15 +2007,15 @@
         <v>224</v>
       </c>
       <c r="G45" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.11160714285714286</v>
       </c>
       <c r="H45" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.12620535714285713</v>
       </c>
       <c r="I45" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-0.13079999999999997</v>
       </c>
       <c r="J45" t="s">
@@ -2030,15 +2042,15 @@
         <v>181</v>
       </c>
       <c r="G46" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.11049723756906077</v>
       </c>
       <c r="H46" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.13458563535911602</v>
       </c>
       <c r="I46" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-0.21799999999999997</v>
       </c>
       <c r="J46" t="s">
@@ -2065,15 +2077,15 @@
         <v>190</v>
       </c>
       <c r="G47" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.11052631578947368</v>
       </c>
       <c r="H47" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.16026315789473683</v>
       </c>
       <c r="I47" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-0.44999999999999996</v>
       </c>
       <c r="J47" t="s">
@@ -2100,15 +2112,15 @@
         <v>266</v>
       </c>
       <c r="G48" s="3">
-        <f t="shared" ref="G48:G55" si="7">D48/F48</f>
+        <f t="shared" ref="G48:G58" si="9">D48/F48</f>
         <v>0.11654135338345864</v>
       </c>
       <c r="H48" s="3">
-        <f t="shared" ref="H48:H55" si="8">E48/F48</f>
+        <f t="shared" ref="H48:H58" si="10">E48/F48</f>
         <v>0.21721804511278195</v>
       </c>
       <c r="I48" s="8">
-        <f t="shared" ref="I48:I55" si="9">(D48-E48)/D48</f>
+        <f t="shared" ref="I48:I58" si="11">(D48-E48)/D48</f>
         <v>-0.8638709677419355</v>
       </c>
       <c r="J48" t="s">
@@ -2135,15 +2147,15 @@
         <v>251</v>
       </c>
       <c r="G49" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.10756972111553785</v>
       </c>
       <c r="H49" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.14533864541832667</v>
       </c>
       <c r="I49" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-0.35111111111111099</v>
       </c>
     </row>
@@ -2167,15 +2179,15 @@
         <v>221</v>
       </c>
       <c r="G50" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.10407239819004525</v>
       </c>
       <c r="H50" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>9.710407239819005E-2</v>
       </c>
       <c r="I50" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>6.6956521739130401E-2</v>
       </c>
     </row>
@@ -2199,15 +2211,15 @@
         <v>220</v>
       </c>
       <c r="G51" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.11363636363636363</v>
       </c>
       <c r="H51" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.12095454545454545</v>
       </c>
       <c r="I51" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-6.4399999999999971E-2</v>
       </c>
     </row>
@@ -2231,15 +2243,15 @@
         <v>135</v>
       </c>
       <c r="G52" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.15555555555555556</v>
       </c>
       <c r="H52" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.18192592592592591</v>
       </c>
       <c r="I52" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-0.16952380952380947</v>
       </c>
     </row>
@@ -2263,15 +2275,15 @@
         <v>170</v>
       </c>
       <c r="G53" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.14705882352941177</v>
       </c>
       <c r="H53" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.1552941176470588</v>
       </c>
       <c r="I53" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-5.5999999999999946E-2</v>
       </c>
       <c r="J53" t="s">
@@ -2298,59 +2310,332 @@
         <v>210</v>
       </c>
       <c r="G54" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.12380952380952381</v>
       </c>
       <c r="H54" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.13123809523809524</v>
       </c>
       <c r="I54" s="5">
+        <f t="shared" si="11"/>
+        <v>-5.9999999999999949E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="B55" s="1">
+        <v>-5.95</v>
+      </c>
+      <c r="C55" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="D55" s="1">
+        <v>28</v>
+      </c>
+      <c r="E55" s="1">
+        <v>34</v>
+      </c>
+      <c r="F55" s="1">
+        <v>169</v>
+      </c>
+      <c r="G55" s="4">
         <f t="shared" si="9"/>
-        <v>-5.9999999999999949E-2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A55">
+        <v>0.16568047337278108</v>
+      </c>
+      <c r="H55" s="4">
+        <f t="shared" si="10"/>
+        <v>0.20118343195266272</v>
+      </c>
+      <c r="I55" s="7">
+        <f t="shared" si="11"/>
+        <v>-0.21428571428571427</v>
+      </c>
+      <c r="J55" s="1"/>
+    </row>
+    <row r="56" spans="1:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>0.09</v>
+      </c>
+      <c r="B56">
+        <v>0.25</v>
+      </c>
+      <c r="C56">
+        <v>0.25</v>
+      </c>
+      <c r="D56">
+        <v>38</v>
+      </c>
+      <c r="E56">
+        <v>53.19</v>
+      </c>
+      <c r="F56">
+        <v>322</v>
+      </c>
+      <c r="G56" s="3">
+        <f t="shared" si="9"/>
+        <v>0.11801242236024845</v>
+      </c>
+      <c r="H56" s="3">
+        <f t="shared" si="10"/>
+        <v>0.16518633540372671</v>
+      </c>
+      <c r="I56" s="5">
+        <f t="shared" si="11"/>
+        <v>-0.39973684210526311</v>
+      </c>
+      <c r="J56" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>0.04</v>
+      </c>
+      <c r="B57">
         <v>0.2</v>
       </c>
-      <c r="B55">
-        <v>-5.95</v>
-      </c>
-      <c r="C55">
-        <v>0.25</v>
-      </c>
-      <c r="D55">
+      <c r="C57">
+        <v>0.25</v>
+      </c>
+      <c r="D57">
+        <v>32</v>
+      </c>
+      <c r="E57">
+        <v>36.69</v>
+      </c>
+      <c r="F57">
+        <v>278</v>
+      </c>
+      <c r="G57" s="3">
+        <f t="shared" si="9"/>
+        <v>0.11510791366906475</v>
+      </c>
+      <c r="H57" s="3">
+        <f t="shared" si="10"/>
+        <v>0.13197841726618703</v>
+      </c>
+      <c r="I57" s="5">
+        <f t="shared" si="11"/>
+        <v>-0.14656249999999993</v>
+      </c>
+      <c r="J57" t="s">
         <v>28</v>
       </c>
-      <c r="E55">
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>0.04</v>
+      </c>
+      <c r="B58">
+        <v>0.2</v>
+      </c>
+      <c r="C58">
+        <v>0.25</v>
+      </c>
+      <c r="D58">
+        <v>32</v>
+      </c>
+      <c r="E58">
+        <v>24.61</v>
+      </c>
+      <c r="F58">
+        <v>240</v>
+      </c>
+      <c r="G58" s="3">
+        <f t="shared" si="9"/>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="H58" s="3">
+        <f t="shared" si="10"/>
+        <v>0.10254166666666667</v>
+      </c>
+      <c r="I58" s="5">
+        <f t="shared" si="11"/>
+        <v>0.23093750000000002</v>
+      </c>
+      <c r="J58" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>0.04</v>
+      </c>
+      <c r="B59">
+        <v>0.2</v>
+      </c>
+      <c r="C59">
+        <v>0.25</v>
+      </c>
+      <c r="D59">
+        <v>36</v>
+      </c>
+      <c r="E59">
+        <v>35.869999999999997</v>
+      </c>
+      <c r="F59">
+        <v>288</v>
+      </c>
+      <c r="G59" s="3">
+        <f t="shared" ref="G59:G66" si="12">D59/F59</f>
+        <v>0.125</v>
+      </c>
+      <c r="H59" s="3">
+        <f t="shared" ref="H59:H66" si="13">E59/F59</f>
+        <v>0.1245486111111111</v>
+      </c>
+      <c r="I59" s="5">
+        <f t="shared" ref="I59:I66" si="14">(D59-E59)/D59</f>
+        <v>3.6111111111111821E-3</v>
+      </c>
+      <c r="J59" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>0.04</v>
+      </c>
+      <c r="B60">
+        <v>0.2</v>
+      </c>
+      <c r="C60">
+        <v>0.25</v>
+      </c>
+      <c r="D60">
+        <v>29</v>
+      </c>
+      <c r="E60">
+        <v>29.2</v>
+      </c>
+      <c r="F60">
+        <v>218</v>
+      </c>
+      <c r="G60" s="3">
+        <f t="shared" si="12"/>
+        <v>0.13302752293577982</v>
+      </c>
+      <c r="H60" s="3">
+        <f t="shared" si="13"/>
+        <v>0.13394495412844037</v>
+      </c>
+      <c r="I60" s="5">
+        <f t="shared" si="14"/>
+        <v>-6.8965517241379067E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>0.04</v>
+      </c>
+      <c r="B61">
+        <v>0.2</v>
+      </c>
+      <c r="C61">
+        <v>0.25</v>
+      </c>
+      <c r="D61">
+        <v>33</v>
+      </c>
+      <c r="E61">
+        <v>33.909999999999997</v>
+      </c>
+      <c r="F61">
+        <v>259</v>
+      </c>
+      <c r="G61" s="3">
+        <f t="shared" si="12"/>
+        <v>0.12741312741312741</v>
+      </c>
+      <c r="H61" s="3">
+        <f t="shared" si="13"/>
+        <v>0.13092664092664091</v>
+      </c>
+      <c r="I61" s="5">
+        <f t="shared" si="14"/>
+        <v>-2.7575757575757472E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D62">
         <v>34</v>
       </c>
-      <c r="F55">
-        <v>169</v>
-      </c>
-      <c r="G55" s="3">
-        <f t="shared" si="7"/>
-        <v>0.16568047337278108</v>
-      </c>
-      <c r="H55" s="3">
-        <f t="shared" si="8"/>
-        <v>0.20118343195266272</v>
-      </c>
-      <c r="I55" s="5">
-        <f t="shared" si="9"/>
-        <v>-0.21428571428571427</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A56">
-        <v>0.2</v>
-      </c>
-      <c r="B56">
-        <v>-5.95</v>
-      </c>
-      <c r="C56">
-        <v>0.25</v>
+      <c r="E62">
+        <v>9.75</v>
+      </c>
+      <c r="F62">
+        <v>65</v>
+      </c>
+      <c r="G62" s="3">
+        <f t="shared" si="12"/>
+        <v>0.52307692307692311</v>
+      </c>
+      <c r="H62" s="3">
+        <f t="shared" si="13"/>
+        <v>0.15</v>
+      </c>
+      <c r="I62" s="5">
+        <f t="shared" si="14"/>
+        <v>0.71323529411764708</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G63" s="3" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H63" s="3" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I63" s="5" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G64" s="3" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H64" s="3" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I64" s="5" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="65" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G65" s="3" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H65" s="3" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I65" s="5" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="66" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G66" s="3" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H66" s="3" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I66" s="5" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>